<commit_message>
EQUIPOS Y JUGADORES CARGADOS
carque todo los datos, y arregle que se guardaban doble
</commit_message>
<xml_diff>
--- a/INFORME TORNEO DE FÚTBOL.xlsx
+++ b/INFORME TORNEO DE FÚTBOL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa_a\Documents\UTN\2DO CUATRIMESTRE\Laboratorio de computacion 2\LAB-2---PROYECTO-INTEGRADOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF5EE45-466C-4191-BCBB-94307175C6F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4A1694-6CEA-4AA9-845C-F6F143650ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{C1A6ECE5-3B1A-4512-B0FD-82BD273B7B69}"/>
+    <workbookView xWindow="15360" yWindow="1605" windowWidth="9885" windowHeight="10440" xr2:uid="{C1A6ECE5-3B1A-4512-B0FD-82BD273B7B69}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="238">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -55,9 +55,6 @@
     <t>RIVER</t>
   </si>
   <si>
-    <t>RACING CLUB</t>
-  </si>
-  <si>
     <t>INDEPENDIENTE</t>
   </si>
   <si>
@@ -746,6 +743,18 @@
   </si>
   <si>
     <t>}</t>
+  </si>
+  <si>
+    <t>RACING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sebastian </t>
+  </si>
+  <si>
+    <t>Nestor Alejandro</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC2D622-994C-4FF3-84B5-F6BC94220F4D}">
   <dimension ref="A1:R211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,10 +1165,10 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1170,39 +1179,39 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
@@ -1245,10 +1254,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>234</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4">
@@ -1257,7 +1266,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1265,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4">
@@ -1274,36 +1283,36 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="H6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="O6" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4">
@@ -1338,10 +1347,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4">
@@ -1376,10 +1385,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4">
@@ -1414,10 +1423,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4">
@@ -1452,7 +1461,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H11" s="4">
         <v>1</v>
@@ -1533,7 +1542,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1544,40 +1553,40 @@
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
@@ -1587,22 +1596,22 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="K16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="7">
         <v>2</v>
@@ -1612,22 +1621,22 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="K17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="7">
         <v>3</v>
@@ -1637,22 +1646,22 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="K18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="7">
         <v>4</v>
@@ -1662,22 +1671,22 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="K19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="7">
         <v>5</v>
@@ -1687,43 +1696,43 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="K20" t="s">
+        <v>206</v>
+      </c>
+      <c r="L20" t="s">
         <v>207</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>208</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>209</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>210</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>211</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>212</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>213</v>
-      </c>
-      <c r="R20" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="7">
         <v>6</v>
@@ -1736,16 +1745,16 @@
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="7">
         <v>7</v>
@@ -1758,16 +1767,16 @@
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="7">
         <v>8</v>
@@ -1777,22 +1786,22 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="K23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="7">
         <v>9</v>
@@ -1802,22 +1811,22 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="K24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="7">
         <v>10</v>
@@ -1827,22 +1836,22 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="K25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <f>A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="7">
         <v>11</v>
@@ -1858,13 +1867,13 @@
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="7">
         <v>1</v>
@@ -1874,7 +1883,7 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="K27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -1883,13 +1892,13 @@
         <v>2</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="7">
         <v>2</v>
@@ -1905,13 +1914,13 @@
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="7">
         <v>3</v>
@@ -1927,13 +1936,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="7">
         <v>4</v>
@@ -1943,7 +1952,7 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="K30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -1952,13 +1961,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" s="7">
         <v>5</v>
@@ -1968,7 +1977,7 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="K31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -1977,13 +1986,13 @@
         <v>2</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32" s="7">
         <v>6</v>
@@ -1999,13 +2008,13 @@
         <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="D33" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" s="7">
         <v>7</v>
@@ -2021,13 +2030,13 @@
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E34" s="7">
         <v>8</v>
@@ -2037,7 +2046,7 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="K34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2046,13 +2055,13 @@
         <v>2</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>145</v>
-      </c>
       <c r="D35" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="7">
         <v>9</v>
@@ -2062,7 +2071,7 @@
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="K35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2071,13 +2080,13 @@
         <v>2</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="D36" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" s="7">
         <v>10</v>
@@ -2087,7 +2096,7 @@
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="K36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2096,13 +2105,13 @@
         <v>2</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37" s="7">
         <v>11</v>
@@ -2112,22 +2121,22 @@
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="K37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E38" s="7">
         <v>1</v>
@@ -2137,22 +2146,22 @@
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="K38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="7">
         <v>2</v>
@@ -2165,16 +2174,16 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="D40" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E40" s="7">
         <v>3</v>
@@ -2184,22 +2193,22 @@
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="K40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="D41" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E41" s="7">
         <v>4</v>
@@ -2209,22 +2218,22 @@
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="K41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="D42" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E42" s="7">
         <v>5</v>
@@ -2234,22 +2243,22 @@
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="K42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E43" s="7">
         <v>6</v>
@@ -2262,16 +2271,16 @@
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="D44" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E44" s="7">
         <v>7</v>
@@ -2281,22 +2290,22 @@
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="K44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="D45" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E45" s="7">
         <v>8</v>
@@ -2306,22 +2315,22 @@
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="K45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>165</v>
-      </c>
       <c r="D46" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E46" s="7">
         <v>9</v>
@@ -2331,22 +2340,22 @@
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="K46" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E47" s="7">
         <v>10</v>
@@ -2356,22 +2365,22 @@
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="K47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <f>A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="D48" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E48" s="7">
         <v>11</v>
@@ -2387,13 +2396,13 @@
         <v>4</v>
       </c>
       <c r="B49" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>170</v>
-      </c>
       <c r="D49" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E49" s="7">
         <v>1</v>
@@ -2403,7 +2412,7 @@
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="K49" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2412,13 +2421,13 @@
         <v>4</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E50" s="7">
         <v>2</v>
@@ -2428,7 +2437,7 @@
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="K50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2437,13 +2446,13 @@
         <v>4</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E51" s="7">
         <v>3</v>
@@ -2459,13 +2468,13 @@
         <v>4</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>174</v>
-      </c>
       <c r="D52" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E52" s="7">
         <v>4</v>
@@ -2475,7 +2484,7 @@
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="K52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2484,13 +2493,13 @@
         <v>4</v>
       </c>
       <c r="B53" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>176</v>
-      </c>
       <c r="D53" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E53" s="7">
         <v>5</v>
@@ -2500,7 +2509,7 @@
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="K53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2509,13 +2518,13 @@
         <v>4</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>178</v>
-      </c>
       <c r="D54" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E54" s="7">
         <v>6</v>
@@ -2525,7 +2534,7 @@
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="K54" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2534,13 +2543,13 @@
         <v>4</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E55" s="7">
         <v>7</v>
@@ -2556,13 +2565,13 @@
         <v>4</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>181</v>
-      </c>
       <c r="D56" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E56" s="7">
         <v>8</v>
@@ -2578,13 +2587,13 @@
         <v>4</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>183</v>
-      </c>
       <c r="D57" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E57" s="7">
         <v>9</v>
@@ -2600,13 +2609,13 @@
         <v>4</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E58" s="7">
         <v>10</v>
@@ -2622,13 +2631,13 @@
         <v>4</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E59" s="7">
         <v>11</v>
@@ -2641,16 +2650,16 @@
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E60" s="7">
         <v>1</v>
@@ -2663,16 +2672,16 @@
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>188</v>
-      </c>
       <c r="D61" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E61" s="7">
         <v>2</v>
@@ -2685,16 +2694,16 @@
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E62" s="7">
         <v>3</v>
@@ -2707,16 +2716,16 @@
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>191</v>
-      </c>
       <c r="D63" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E63" s="7">
         <v>4</v>
@@ -2729,16 +2738,16 @@
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E64" s="7">
         <v>5</v>
@@ -2751,16 +2760,16 @@
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E65" s="7">
         <v>6</v>
@@ -2773,16 +2782,16 @@
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E66" s="7">
         <v>7</v>
@@ -2795,16 +2804,16 @@
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E67" s="7">
         <v>8</v>
@@ -2817,16 +2826,16 @@
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>197</v>
-      </c>
       <c r="D68" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E68" s="7">
         <v>9</v>
@@ -2839,16 +2848,16 @@
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E69" s="7">
         <v>10</v>
@@ -2861,16 +2870,16 @@
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <f>A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E70" s="7">
         <v>11</v>
@@ -2883,16 +2892,16 @@
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="D71" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="E71" s="7">
         <v>1</v>
@@ -2905,16 +2914,16 @@
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E72" s="7">
         <v>2</v>
@@ -2927,16 +2936,16 @@
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E73" s="7">
         <v>3</v>
@@ -2949,16 +2958,16 @@
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="D74" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E74" s="7">
         <v>4</v>
@@ -2971,16 +2980,16 @@
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="D75" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E75" s="7">
         <v>5</v>
@@ -2993,16 +3002,16 @@
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="E76" s="7">
         <v>6</v>
@@ -3015,16 +3024,16 @@
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E77" s="7">
         <v>7</v>
@@ -3037,16 +3046,16 @@
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="D78" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E78" s="7">
         <v>8</v>
@@ -3059,16 +3068,16 @@
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="D79" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="E79" s="7">
         <v>9</v>
@@ -3081,16 +3090,16 @@
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E80" s="7">
         <v>10</v>
@@ -3103,16 +3112,16 @@
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <f>A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E81" s="7">
         <v>11</v>
@@ -3125,16 +3134,16 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="D82" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E82" s="7">
         <v>1</v>
@@ -3147,16 +3156,16 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B83" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C83" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="D83" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E83" s="7">
         <v>2</v>
@@ -3169,16 +3178,16 @@
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B84" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="D84" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E84" s="7">
         <v>3</v>
@@ -3191,16 +3200,16 @@
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E85" s="7">
         <v>4</v>
@@ -3213,16 +3222,16 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E86" s="7">
         <v>5</v>
@@ -3235,16 +3244,16 @@
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B87" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="D87" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E87" s="7">
         <v>6</v>
@@ -3257,16 +3266,16 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B88" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C88" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="D88" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E88" s="7">
         <v>7</v>
@@ -3279,16 +3288,16 @@
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B89" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="D89" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E89" s="7">
         <v>8</v>
@@ -3301,16 +3310,16 @@
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E90" s="7">
         <v>9</v>
@@ -3323,16 +3332,16 @@
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B91" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="D91" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E91" s="7">
         <v>10</v>
@@ -3345,16 +3354,16 @@
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <f>A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B92" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C92" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="D92" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E92" s="7">
         <v>11</v>
@@ -3367,16 +3376,16 @@
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E93" s="7">
         <v>1</v>
@@ -3389,16 +3398,16 @@
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C94" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="D94" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E94" s="7">
         <v>2</v>
@@ -3411,16 +3420,16 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E95" s="7">
         <v>3</v>
@@ -3433,16 +3442,16 @@
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B96" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C96" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C96" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="D96" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E96" s="7">
         <v>4</v>
@@ -3455,16 +3464,16 @@
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B97" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C97" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C97" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="D97" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E97" s="7">
         <v>5</v>
@@ -3477,16 +3486,16 @@
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B98" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C98" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C98" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="D98" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E98" s="7">
         <v>6</v>
@@ -3499,16 +3508,16 @@
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B99" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C99" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C99" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="D99" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E99" s="7">
         <v>7</v>
@@ -3521,16 +3530,16 @@
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B100" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C100" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="D100" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E100" s="7">
         <v>8</v>
@@ -3543,16 +3552,16 @@
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B101" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C101" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="D101" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E101" s="7">
         <v>9</v>
@@ -3565,16 +3574,16 @@
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E102" s="7">
         <v>10</v>
@@ -3587,16 +3596,16 @@
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <f>A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E103" s="7">
         <v>11</v>
@@ -4815,7 +4824,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4826,40 +4835,40 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" t="s">
         <v>109</v>
       </c>
-      <c r="C3" t="s">
-        <v>110</v>
-      </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -4868,16 +4877,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
         <v>111</v>
       </c>
-      <c r="C4" t="s">
-        <v>112</v>
-      </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -4886,16 +4895,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
         <v>113</v>
       </c>
-      <c r="C5" t="s">
-        <v>114</v>
-      </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -4904,16 +4913,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" t="s">
         <v>115</v>
       </c>
-      <c r="C6" t="s">
-        <v>116</v>
-      </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -4922,16 +4931,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
         <v>117</v>
       </c>
-      <c r="C7" t="s">
-        <v>118</v>
-      </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
@@ -4940,16 +4949,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
         <v>119</v>
       </c>
-      <c r="C8" t="s">
-        <v>120</v>
-      </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
@@ -4958,16 +4967,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
         <v>121</v>
       </c>
-      <c r="C9" t="s">
-        <v>122</v>
-      </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
@@ -4976,16 +4985,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -4994,16 +5003,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" t="s">
         <v>125</v>
       </c>
-      <c r="C11" t="s">
-        <v>126</v>
-      </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -5012,16 +5021,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -5030,16 +5039,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2">
         <v>11</v>
@@ -5065,7 +5074,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5076,25 +5085,25 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5103,13 +5112,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
         <v>129</v>
       </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -5121,13 +5130,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" t="s">
         <v>131</v>
       </c>
-      <c r="C4" t="s">
-        <v>132</v>
-      </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -5139,13 +5148,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
         <v>133</v>
       </c>
-      <c r="C5" t="s">
-        <v>134</v>
-      </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -5157,13 +5166,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" t="s">
         <v>135</v>
       </c>
-      <c r="C6" t="s">
-        <v>136</v>
-      </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -5175,13 +5184,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" t="s">
         <v>137</v>
       </c>
-      <c r="C7" t="s">
-        <v>138</v>
-      </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
@@ -5193,13 +5202,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" t="s">
         <v>139</v>
       </c>
-      <c r="C8" t="s">
-        <v>140</v>
-      </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
@@ -5211,13 +5220,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
         <v>141</v>
       </c>
-      <c r="C9" t="s">
-        <v>142</v>
-      </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
@@ -5229,13 +5238,13 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -5247,13 +5256,13 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" t="s">
         <v>144</v>
       </c>
-      <c r="C11" t="s">
-        <v>145</v>
-      </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -5265,13 +5274,13 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
         <v>146</v>
       </c>
-      <c r="C12" t="s">
-        <v>147</v>
-      </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -5283,13 +5292,13 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2">
         <v>11</v>
@@ -5305,7 +5314,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5316,7 +5325,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5327,40 +5336,40 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -5369,16 +5378,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" t="s">
         <v>151</v>
       </c>
-      <c r="C4" t="s">
-        <v>152</v>
-      </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -5387,16 +5396,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
         <v>153</v>
       </c>
-      <c r="C5" t="s">
-        <v>154</v>
-      </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -5405,16 +5414,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" t="s">
         <v>155</v>
       </c>
-      <c r="C6" t="s">
-        <v>156</v>
-      </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -5423,16 +5432,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" t="s">
         <v>157</v>
       </c>
-      <c r="C7" t="s">
-        <v>158</v>
-      </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
@@ -5441,16 +5450,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
@@ -5459,16 +5468,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" t="s">
         <v>160</v>
       </c>
-      <c r="C9" t="s">
-        <v>161</v>
-      </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
@@ -5477,16 +5486,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" t="s">
         <v>162</v>
       </c>
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -5495,16 +5504,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" t="s">
         <v>164</v>
       </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -5513,16 +5522,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -5531,16 +5540,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" t="s">
         <v>167</v>
       </c>
-      <c r="C13" t="s">
-        <v>168</v>
-      </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2">
         <v>11</v>
@@ -5553,257 +5562,6 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0966C69-8D71-4A1B-9E4D-E57E600DFBDF}">
-  <dimension ref="A1:I13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <f>General!A6</f>
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>185</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="2">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A500CBF1-B1F9-466C-B894-57584F4EDDF7}">
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5817,7 +5575,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -5828,40 +5586,291 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <f>General!A6</f>
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="2">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A500CBF1-B1F9-466C-B894-57584F4EDDF7}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -5870,16 +5879,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" t="s">
         <v>187</v>
       </c>
-      <c r="C4" t="s">
-        <v>188</v>
-      </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -5888,16 +5897,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -5906,16 +5915,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" t="s">
         <v>190</v>
       </c>
-      <c r="C6" t="s">
-        <v>191</v>
-      </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -5924,16 +5933,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
@@ -5942,16 +5951,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
@@ -5960,16 +5969,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
@@ -5978,16 +5987,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -5996,16 +6005,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" t="s">
         <v>196</v>
       </c>
-      <c r="C11" t="s">
-        <v>197</v>
-      </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -6014,16 +6023,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -6032,16 +6041,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A7</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2">
         <v>11</v>
@@ -6057,17 +6066,18 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6078,40 +6088,40 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -6120,16 +6130,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -6138,16 +6148,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -6156,16 +6166,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -6174,16 +6184,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
@@ -6192,16 +6202,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
@@ -6210,16 +6220,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>236</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
@@ -6228,16 +6238,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" t="s">
-        <v>57</v>
-      </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -6246,16 +6256,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>59</v>
-      </c>
-      <c r="D11" t="s">
-        <v>60</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -6264,16 +6274,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -6282,16 +6292,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A8</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2">
         <v>11</v>
@@ -6307,17 +6317,18 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6328,40 +6339,40 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -6370,16 +6381,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -6388,16 +6399,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
         <v>69</v>
       </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -6406,16 +6417,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -6424,16 +6435,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>237</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
@@ -6442,16 +6453,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
-        <v>76</v>
-      </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
@@ -6460,16 +6471,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" t="s">
-        <v>78</v>
-      </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
@@ -6478,16 +6489,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
         <v>79</v>
       </c>
-      <c r="C10" t="s">
-        <v>80</v>
-      </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -6496,16 +6507,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -6514,16 +6525,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
         <v>82</v>
       </c>
-      <c r="C12" t="s">
-        <v>83</v>
-      </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -6532,16 +6543,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A9</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
         <v>84</v>
       </c>
-      <c r="C13" t="s">
-        <v>85</v>
-      </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2">
         <v>11</v>
@@ -6567,7 +6578,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6578,40 +6589,40 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -6620,16 +6631,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
-        <v>92</v>
-      </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -6638,16 +6649,16 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -6656,16 +6667,16 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" t="s">
         <v>95</v>
       </c>
-      <c r="C6" t="s">
-        <v>96</v>
-      </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
@@ -6674,16 +6685,16 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
         <v>97</v>
       </c>
-      <c r="C7" t="s">
-        <v>98</v>
-      </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
@@ -6692,16 +6703,16 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" t="s">
         <v>99</v>
       </c>
-      <c r="C8" t="s">
-        <v>100</v>
-      </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
@@ -6710,16 +6721,16 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
         <v>101</v>
       </c>
-      <c r="C9" t="s">
-        <v>102</v>
-      </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
@@ -6728,16 +6739,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" t="s">
         <v>103</v>
       </c>
-      <c r="C10" t="s">
-        <v>104</v>
-      </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>8</v>
@@ -6746,16 +6757,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
         <v>105</v>
       </c>
-      <c r="C11" t="s">
-        <v>106</v>
-      </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2">
         <v>9</v>
@@ -6764,16 +6775,16 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
@@ -6782,16 +6793,16 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="2">
         <v>11</v>

</xml_diff>

<commit_message>
AGUS LA CONCHA DE TU MADRE
</commit_message>
<xml_diff>
--- a/INFORME TORNEO DE FÚTBOL.xlsx
+++ b/INFORME TORNEO DE FÚTBOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa_a\Documents\UTN\2DO CUATRIMESTRE\Laboratorio de computacion 2\LAB-2---PROYECTO-INTEGRADOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69763F82-6377-49D6-A2B7-B716EC96FD4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E77FB2-40EC-432B-B311-7F64989B7E81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10410" yWindow="0" windowWidth="9885" windowHeight="10440" xr2:uid="{C1A6ECE5-3B1A-4512-B0FD-82BD273B7B69}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="259">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -812,6 +812,12 @@
   </si>
   <si>
     <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>falta validar los ingresos en los penales</t>
+  </si>
+  <si>
+    <t>falta emproligar ver resultados</t>
   </si>
 </sst>
 </file>
@@ -1348,7 +1354,7 @@
   <dimension ref="A1:AA211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3594,6 +3600,9 @@
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
+      <c r="K64" t="s">
+        <v>258</v>
+      </c>
       <c r="Z64" s="12">
         <v>58</v>
       </c>
@@ -3622,6 +3631,9 @@
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
+      <c r="K65" t="s">
+        <v>257</v>
+      </c>
       <c r="Z65" s="12">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
sorteo solucionado, hay que cargar todo de nuevo jaja
</commit_message>
<xml_diff>
--- a/INFORME TORNEO DE FÚTBOL.xlsx
+++ b/INFORME TORNEO DE FÚTBOL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa_a\Documents\UTN\2DO CUATRIMESTRE\Laboratorio de computacion 2\LAB-2---PROYECTO-INTEGRADOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A16E727-46CE-45CB-92F8-5094D0CA8864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8095D103-A51F-421A-A2E8-C5ADB0442859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C1A6ECE5-3B1A-4512-B0FD-82BD273B7B69}"/>
+    <workbookView xWindow="8145" yWindow="480" windowWidth="9885" windowHeight="10440" xr2:uid="{C1A6ECE5-3B1A-4512-B0FD-82BD273B7B69}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="262">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -1362,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC2D622-994C-4FF3-84B5-F6BC94220F4D}">
   <dimension ref="A1:AK211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1548,7 @@
       <c r="P6" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AD6" t="s">
         <v>261</v>
       </c>
       <c r="AF6" t="s">
@@ -1616,11 +1616,14 @@
       <c r="AA7">
         <v>0</v>
       </c>
-      <c r="AD7">
+      <c r="AC7">
         <v>0</v>
       </c>
-      <c r="AE7" s="4">
-        <v>7</v>
+      <c r="AD7" s="4">
+        <v>4</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="AF7" s="4">
         <v>1</v>
@@ -1699,11 +1702,14 @@
       <c r="AA8">
         <v>1</v>
       </c>
-      <c r="AD8">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="4">
-        <v>2</v>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>8</v>
+      </c>
+      <c r="AE8" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="AF8" s="4">
         <v>1</v>
@@ -1782,11 +1788,14 @@
       <c r="AA9">
         <v>2</v>
       </c>
-      <c r="AD9">
+      <c r="AC9">
         <v>2</v>
       </c>
-      <c r="AE9" s="4">
-        <v>5</v>
+      <c r="AD9" s="4">
+        <v>7</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>233</v>
       </c>
       <c r="AF9" s="4">
         <v>1</v>
@@ -1865,10 +1874,13 @@
       <c r="AA10">
         <v>3</v>
       </c>
-      <c r="AD10">
+      <c r="AC10">
         <v>3</v>
       </c>
-      <c r="AE10" s="4">
+      <c r="AD10" s="4">
+        <v>5</v>
+      </c>
+      <c r="AE10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="AF10" s="4">
@@ -1936,11 +1948,14 @@
       <c r="AA11">
         <v>4</v>
       </c>
-      <c r="AD11">
+      <c r="AC11">
         <v>4</v>
       </c>
-      <c r="AE11" s="4">
+      <c r="AD11" s="4">
         <v>6</v>
+      </c>
+      <c r="AE11" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="AF11" s="4">
         <v>1</v>
@@ -2004,11 +2019,14 @@
       <c r="AA12">
         <v>5</v>
       </c>
-      <c r="AD12">
+      <c r="AC12">
         <v>5</v>
       </c>
-      <c r="AE12" s="4">
-        <v>8</v>
+      <c r="AD12" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE12" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="AF12" s="4">
         <v>1</v>
@@ -2072,11 +2090,14 @@
       <c r="AA13">
         <v>6</v>
       </c>
-      <c r="AD13">
+      <c r="AC13">
         <v>6</v>
       </c>
-      <c r="AE13" s="4">
+      <c r="AD13" s="4">
         <v>3</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="AF13" s="4">
         <v>1</v>
@@ -2113,11 +2134,14 @@
       <c r="AA14">
         <v>7</v>
       </c>
-      <c r="AD14">
+      <c r="AC14">
         <v>7</v>
       </c>
-      <c r="AE14" s="4">
-        <v>1</v>
+      <c r="AD14" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="AF14" s="4">
         <v>1</v>
@@ -8045,7 +8069,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
EQUIPOS Y JUG CARGADOS
</commit_message>
<xml_diff>
--- a/INFORME TORNEO DE FÚTBOL.xlsx
+++ b/INFORME TORNEO DE FÚTBOL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa_a\Documents\UTN\2DO CUATRIMESTRE\Laboratorio de computacion 2\LAB-2---PROYECTO-INTEGRADOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74564A13-385D-4324-8066-1225375451A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC16E64-B5C3-44BC-ABC4-A2656FE277B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C1A6ECE5-3B1A-4512-B0FD-82BD273B7B69}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="263">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -827,6 +827,9 @@
   </si>
   <si>
     <t>vecAleatorio</t>
+  </si>
+  <si>
+    <t>verificar que al cargar los jugadores el numero de camisate ya no se haya usado</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1046,6 +1049,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC2D622-994C-4FF3-84B5-F6BC94220F4D}">
   <dimension ref="A1:AK211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1430,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
@@ -1462,7 +1466,7 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
@@ -1483,7 +1487,7 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>233</v>
@@ -1507,7 +1511,7 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -1560,7 +1564,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
@@ -1646,7 +1650,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>63</v>
@@ -1732,7 +1736,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>35</v>
@@ -1818,7 +1822,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>36</v>
@@ -2224,7 +2228,7 @@
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>108</v>
@@ -2279,7 +2283,7 @@
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>110</v>
@@ -2334,7 +2338,7 @@
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>112</v>
@@ -2389,7 +2393,7 @@
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>114</v>
@@ -2444,7 +2448,7 @@
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>116</v>
@@ -2520,7 +2524,7 @@
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>118</v>
@@ -2572,7 +2576,7 @@
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>120</v>
@@ -2622,7 +2626,7 @@
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>76</v>
@@ -2675,7 +2679,7 @@
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>124</v>
@@ -2728,7 +2732,7 @@
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>114</v>
@@ -2781,7 +2785,7 @@
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <f>A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>127</v>
@@ -2831,7 +2835,7 @@
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>128</v>
@@ -2884,7 +2888,7 @@
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>130</v>
@@ -2934,7 +2938,7 @@
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>132</v>
@@ -2984,7 +2988,7 @@
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>134</v>
@@ -3037,7 +3041,7 @@
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>136</v>
@@ -3090,7 +3094,7 @@
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>138</v>
@@ -3140,7 +3144,7 @@
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>140</v>
@@ -3190,7 +3194,7 @@
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>118</v>
@@ -3225,7 +3229,7 @@
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>143</v>
@@ -3260,7 +3264,7 @@
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>145</v>
@@ -3295,7 +3299,7 @@
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <f>A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>38</v>
@@ -3330,7 +3334,7 @@
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>149</v>
@@ -3361,7 +3365,7 @@
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>150</v>
@@ -3389,7 +3393,7 @@
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>152</v>
@@ -3420,7 +3424,7 @@
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>154</v>
@@ -3451,7 +3455,7 @@
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>156</v>
@@ -3482,7 +3486,7 @@
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>158</v>
@@ -3510,7 +3514,7 @@
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>159</v>
@@ -3541,7 +3545,7 @@
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>161</v>
@@ -3572,7 +3576,7 @@
     <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>163</v>
@@ -3603,7 +3607,7 @@
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>165</v>
@@ -3634,7 +3638,7 @@
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <f>A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>166</v>
@@ -3662,7 +3666,7 @@
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>168</v>
@@ -3693,7 +3697,7 @@
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>170</v>
@@ -3724,7 +3728,7 @@
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>74</v>
@@ -3752,7 +3756,7 @@
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>172</v>
@@ -3783,7 +3787,7 @@
     <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>174</v>
@@ -3814,7 +3818,7 @@
     <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>176</v>
@@ -3845,7 +3849,7 @@
     <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>114</v>
@@ -3873,7 +3877,7 @@
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>179</v>
@@ -3904,7 +3908,7 @@
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>181</v>
@@ -3941,7 +3945,7 @@
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>170</v>
@@ -3969,7 +3973,7 @@
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <f>A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>184</v>
@@ -4010,7 +4014,7 @@
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>53</v>
@@ -4041,7 +4045,7 @@
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>186</v>
@@ -4085,7 +4089,7 @@
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>138</v>
@@ -4151,7 +4155,7 @@
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>189</v>
@@ -4179,7 +4183,7 @@
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>102</v>
@@ -4213,7 +4217,7 @@
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>44</v>
@@ -4247,7 +4251,7 @@
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>193</v>
@@ -4278,7 +4282,7 @@
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>143</v>
@@ -4296,6 +4300,9 @@
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
+      <c r="K67" s="31" t="s">
+        <v>262</v>
+      </c>
       <c r="Z67" s="21">
         <v>61</v>
       </c>
@@ -4306,7 +4313,7 @@
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>195</v>
@@ -4334,7 +4341,7 @@
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>128</v>
@@ -4362,7 +4369,7 @@
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <f>A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>198</v>
@@ -4393,7 +4400,7 @@
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>38</v>
@@ -4421,7 +4428,7 @@
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>41</v>
@@ -4452,7 +4459,7 @@
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>85</v>
@@ -4474,7 +4481,7 @@
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>46</v>
@@ -4496,7 +4503,7 @@
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>48</v>
@@ -4518,7 +4525,7 @@
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>50</v>
@@ -4540,7 +4547,7 @@
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>86</v>
@@ -4562,7 +4569,7 @@
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>55</v>
@@ -4584,7 +4591,7 @@
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>57</v>
@@ -4606,7 +4613,7 @@
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>87</v>
@@ -4628,7 +4635,7 @@
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <f>A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>88</v>
@@ -4650,7 +4657,7 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>64</v>
@@ -4672,7 +4679,7 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>66</v>
@@ -4694,7 +4701,7 @@
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>68</v>
@@ -4716,7 +4723,7 @@
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>72</v>
@@ -4738,7 +4745,7 @@
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>73</v>
@@ -4760,7 +4767,7 @@
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>74</v>
@@ -4782,7 +4789,7 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>76</v>
@@ -4804,7 +4811,7 @@
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>78</v>
@@ -4826,7 +4833,7 @@
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>64</v>
@@ -4848,7 +4855,7 @@
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>81</v>
@@ -4870,7 +4877,7 @@
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <f>A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>83</v>
@@ -4892,7 +4899,7 @@
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>44</v>
@@ -4914,7 +4921,7 @@
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>90</v>
@@ -4936,7 +4943,7 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>93</v>
@@ -4958,7 +4965,7 @@
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>94</v>
@@ -4980,7 +4987,7 @@
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>96</v>
@@ -5002,7 +5009,7 @@
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>98</v>
@@ -5024,7 +5031,7 @@
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>100</v>
@@ -5046,7 +5053,7 @@
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>102</v>
@@ -5068,7 +5075,7 @@
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>104</v>
@@ -5090,7 +5097,7 @@
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>76</v>
@@ -5112,7 +5119,7 @@
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <f>A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>61</v>
@@ -6375,7 +6382,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>108</v>
@@ -6393,7 +6400,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>110</v>
@@ -6411,7 +6418,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>112</v>
@@ -6429,7 +6436,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>114</v>
@@ -6447,7 +6454,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>116</v>
@@ -6465,7 +6472,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>118</v>
@@ -6483,7 +6490,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>120</v>
@@ -6501,7 +6508,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>76</v>
@@ -6519,7 +6526,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>124</v>
@@ -6537,7 +6544,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>114</v>
@@ -6555,7 +6562,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A3</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>127</v>
@@ -6580,7 +6587,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6604,10 +6611,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -6625,7 +6632,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
@@ -6633,17 +6640,17 @@
       <c r="C3" t="s">
         <v>129</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>130</v>
@@ -6651,17 +6658,17 @@
       <c r="C4" t="s">
         <v>131</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>132</v>
@@ -6669,17 +6676,17 @@
       <c r="C5" t="s">
         <v>133</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>134</v>
@@ -6687,17 +6694,17 @@
       <c r="C6" t="s">
         <v>135</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>136</v>
@@ -6705,17 +6712,17 @@
       <c r="C7" t="s">
         <v>137</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>138</v>
@@ -6723,17 +6730,17 @@
       <c r="C8" t="s">
         <v>139</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>140</v>
@@ -6741,17 +6748,17 @@
       <c r="C9" t="s">
         <v>141</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>118</v>
@@ -6759,17 +6766,17 @@
       <c r="C10" t="s">
         <v>142</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>143</v>
@@ -6777,17 +6784,17 @@
       <c r="C11" t="s">
         <v>144</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>145</v>
@@ -6795,17 +6802,17 @@
       <c r="C12" t="s">
         <v>146</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>59</v>
-      </c>
-      <c r="E12" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A4</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
@@ -6813,11 +6820,11 @@
       <c r="C13" t="s">
         <v>147</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
-      </c>
-      <c r="E13" s="2">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -6830,7 +6837,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6855,10 +6862,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -6876,7 +6883,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>149</v>
@@ -6884,17 +6891,17 @@
       <c r="C3" t="s">
         <v>148</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>150</v>
@@ -6902,17 +6909,17 @@
       <c r="C4" t="s">
         <v>151</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>152</v>
@@ -6920,17 +6927,17 @@
       <c r="C5" t="s">
         <v>153</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>154</v>
@@ -6938,17 +6945,17 @@
       <c r="C6" t="s">
         <v>155</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>156</v>
@@ -6956,17 +6963,17 @@
       <c r="C7" t="s">
         <v>157</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>234</v>
@@ -6974,17 +6981,17 @@
       <c r="C8" t="s">
         <v>131</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>159</v>
@@ -6992,17 +6999,17 @@
       <c r="C9" t="s">
         <v>160</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>161</v>
@@ -7010,17 +7017,17 @@
       <c r="C10" t="s">
         <v>162</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
         <v>163</v>
@@ -7028,17 +7035,17 @@
       <c r="C11" t="s">
         <v>164</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>165</v>
@@ -7046,17 +7053,17 @@
       <c r="C12" t="s">
         <v>137</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>59</v>
-      </c>
-      <c r="E12" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A5</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>166</v>
@@ -7064,11 +7071,11 @@
       <c r="C13" t="s">
         <v>167</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
-      </c>
-      <c r="E13" s="2">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -7081,7 +7088,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7105,10 +7112,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -7126,7 +7133,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>168</v>
@@ -7134,17 +7141,17 @@
       <c r="C3" t="s">
         <v>169</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>170</v>
@@ -7152,17 +7159,17 @@
       <c r="C4" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>74</v>
@@ -7170,17 +7177,17 @@
       <c r="C5" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>172</v>
@@ -7188,17 +7195,17 @@
       <c r="C6" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>174</v>
@@ -7206,17 +7213,17 @@
       <c r="C7" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>176</v>
@@ -7224,17 +7231,17 @@
       <c r="C8" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>114</v>
@@ -7242,17 +7249,17 @@
       <c r="C9" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>179</v>
@@ -7260,17 +7267,17 @@
       <c r="C10" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>181</v>
@@ -7278,17 +7285,17 @@
       <c r="C11" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>170</v>
@@ -7296,17 +7303,17 @@
       <c r="C12" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>59</v>
-      </c>
-      <c r="E12" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A6</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>184</v>
@@ -7314,11 +7321,11 @@
       <c r="C13" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
-      </c>
-      <c r="E13" s="2">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -7331,8 +7338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A500CBF1-B1F9-466C-B894-57584F4EDDF7}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7356,10 +7363,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -7377,7 +7384,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
@@ -7385,17 +7392,17 @@
       <c r="C3" t="s">
         <v>185</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>186</v>
@@ -7403,17 +7410,17 @@
       <c r="C4" t="s">
         <v>187</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>138</v>
@@ -7421,17 +7428,17 @@
       <c r="C5" t="s">
         <v>188</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>189</v>
@@ -7439,17 +7446,17 @@
       <c r="C6" t="s">
         <v>190</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>102</v>
@@ -7457,17 +7464,17 @@
       <c r="C7" t="s">
         <v>191</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
@@ -7475,17 +7482,17 @@
       <c r="C8" t="s">
         <v>192</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>193</v>
@@ -7493,17 +7500,17 @@
       <c r="C9" t="s">
         <v>70</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>143</v>
@@ -7511,17 +7518,17 @@
       <c r="C10" t="s">
         <v>194</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>195</v>
@@ -7529,17 +7536,17 @@
       <c r="C11" t="s">
         <v>196</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>128</v>
@@ -7547,17 +7554,17 @@
       <c r="C12" t="s">
         <v>197</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>59</v>
-      </c>
-      <c r="E12" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A7</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>198</v>
@@ -7565,11 +7572,11 @@
       <c r="C13" t="s">
         <v>182</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
-      </c>
-      <c r="E13" s="2">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -7581,8 +7588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D8D03F-6E25-45D1-B31C-B12E671D6F0D}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7607,10 +7614,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -7628,7 +7635,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
@@ -7636,17 +7643,17 @@
       <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>41</v>
@@ -7654,17 +7661,17 @@
       <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>85</v>
@@ -7672,17 +7679,17 @@
       <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>46</v>
@@ -7690,17 +7697,17 @@
       <c r="C6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -7708,17 +7715,17 @@
       <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -7726,17 +7733,17 @@
       <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>235</v>
@@ -7744,17 +7751,17 @@
       <c r="C9" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>55</v>
@@ -7762,17 +7769,17 @@
       <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>57</v>
@@ -7780,17 +7787,17 @@
       <c r="C11" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>87</v>
@@ -7798,17 +7805,17 @@
       <c r="C12" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>59</v>
-      </c>
-      <c r="E12" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A8</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>88</v>
@@ -7816,11 +7823,11 @@
       <c r="C13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
-      </c>
-      <c r="E13" s="2">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -7833,7 +7840,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7858,10 +7865,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -7879,7 +7886,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
@@ -7887,17 +7894,17 @@
       <c r="C3" t="s">
         <v>65</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>66</v>
@@ -7905,17 +7912,17 @@
       <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
@@ -7923,17 +7930,17 @@
       <c r="C5" t="s">
         <v>69</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>72</v>
@@ -7941,17 +7948,17 @@
       <c r="C6" t="s">
         <v>70</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" s="2">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>236</v>
@@ -7959,17 +7966,17 @@
       <c r="C7" t="s">
         <v>71</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>74</v>
@@ -7977,17 +7984,17 @@
       <c r="C8" t="s">
         <v>75</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>52</v>
-      </c>
-      <c r="E8" s="2">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>76</v>
@@ -7995,17 +8002,17 @@
       <c r="C9" t="s">
         <v>77</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>78</v>
@@ -8013,17 +8020,17 @@
       <c r="C10" t="s">
         <v>79</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -8031,17 +8038,17 @@
       <c r="C11" t="s">
         <v>80</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="2">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>81</v>
@@ -8049,17 +8056,17 @@
       <c r="C12" t="s">
         <v>82</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>59</v>
-      </c>
-      <c r="E12" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A9</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
@@ -8067,11 +8074,11 @@
       <c r="C13" t="s">
         <v>84</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
-      </c>
-      <c r="E13" s="2">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -8129,7 +8136,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
@@ -8147,7 +8154,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>90</v>
@@ -8165,7 +8172,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>93</v>
@@ -8183,7 +8190,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>94</v>
@@ -8201,7 +8208,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>96</v>
@@ -8219,7 +8226,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>98</v>
@@ -8237,7 +8244,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>100</v>
@@ -8255,7 +8262,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>102</v>
@@ -8273,7 +8280,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>104</v>
@@ -8291,7 +8298,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>76</v>
@@ -8309,7 +8316,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>General!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>61</v>

</xml_diff>